<commit_message>
Some basic config work in .config
</commit_message>
<xml_diff>
--- a/trunk/txtckr.xlsx
+++ b/trunk/txtckr.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$F$46</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="337">
   <si>
     <t>advisor</t>
   </si>
@@ -898,6 +899,138 @@
   </si>
   <si>
     <t>ALL-ER</t>
+  </si>
+  <si>
+    <t>ABST  - Abstract</t>
+  </si>
+  <si>
+    <t>ADVS  - Audiovisual material</t>
+  </si>
+  <si>
+    <t>ART   - Art Work</t>
+  </si>
+  <si>
+    <t>BILL  - Bill/Resolution[1]</t>
+  </si>
+  <si>
+    <t>BOOK  - Whole book</t>
+  </si>
+  <si>
+    <t>CASE  - Case</t>
+  </si>
+  <si>
+    <t>CHAP  - Book chapter</t>
+  </si>
+  <si>
+    <t>COMP  - Computer program</t>
+  </si>
+  <si>
+    <t>CONF  - Conference proceeding</t>
+  </si>
+  <si>
+    <t>CTLG  - Catalog</t>
+  </si>
+  <si>
+    <t>DATA  - Data file</t>
+  </si>
+  <si>
+    <t>ELEC  - Electronic Citation</t>
+  </si>
+  <si>
+    <t>GEN   - Generic</t>
+  </si>
+  <si>
+    <t>HEAR  - Hearing</t>
+  </si>
+  <si>
+    <t>ICOMM - Internet Communication</t>
+  </si>
+  <si>
+    <t>INPR  - In Press</t>
+  </si>
+  <si>
+    <t>JFULL - Journal (full)</t>
+  </si>
+  <si>
+    <t>JOUR  - Journal</t>
+  </si>
+  <si>
+    <t>MAP   - Map</t>
+  </si>
+  <si>
+    <t>MGZN  - Magazine article</t>
+  </si>
+  <si>
+    <t>MPCT  - Motion picture</t>
+  </si>
+  <si>
+    <t>MUSIC - Music score</t>
+  </si>
+  <si>
+    <t>NEWS  - Newspaper</t>
+  </si>
+  <si>
+    <t>PAMP  - Pamphlet</t>
+  </si>
+  <si>
+    <t>PAT   - Patent</t>
+  </si>
+  <si>
+    <t>PCOMM - Personal communication</t>
+  </si>
+  <si>
+    <t>RPRT  - Report</t>
+  </si>
+  <si>
+    <t>SER   - Serial publication</t>
+  </si>
+  <si>
+    <t>SLIDE - Slide</t>
+  </si>
+  <si>
+    <t>SOUND - Sound recording</t>
+  </si>
+  <si>
+    <t>STAT  - Statute</t>
+  </si>
+  <si>
+    <t>THES  - Thesis/Dissertation</t>
+  </si>
+  <si>
+    <t>UNBILl  - Unenacted bill/resolution[1]</t>
+  </si>
+  <si>
+    <t>UNPB  - Unpublished work</t>
+  </si>
+  <si>
+    <t>VIDEO - Video recording</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>AVM</t>
+  </si>
+  <si>
+    <t>LGL</t>
+  </si>
+  <si>
+    <t>SER</t>
+  </si>
+  <si>
+    <t>MSC</t>
+  </si>
+  <si>
+    <t>PCM</t>
+  </si>
+  <si>
+    <t>MNG</t>
+  </si>
+  <si>
+    <t>ELC</t>
+  </si>
+  <si>
+    <t>IPM</t>
   </si>
 </sst>
 </file>
@@ -913,7 +1046,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -932,6 +1065,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -945,10 +1084,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,7 +1401,7 @@
   <dimension ref="B1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C59"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,8 +1891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D46"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,12 +2466,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:A67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -4021,4 +4164,372 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="G1:G10">
+    <sortCondition ref="G1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing bugs! Working preliminary version
</commit_message>
<xml_diff>
--- a/trunk/txtckr.xlsx
+++ b/trunk/txtckr.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="345">
   <si>
     <t>advisor</t>
   </si>
@@ -1031,6 +1031,30 @@
   </si>
   <si>
     <t>IPM</t>
+  </si>
+  <si>
+    <t>Monograph</t>
+  </si>
+  <si>
+    <t>Intellectual material</t>
+  </si>
+  <si>
+    <t>Electronic data files</t>
+  </si>
+  <si>
+    <t>Legal material</t>
+  </si>
+  <si>
+    <t>Misc general</t>
+  </si>
+  <si>
+    <t>Personal communications</t>
+  </si>
+  <si>
+    <t>Serial publications</t>
+  </si>
+  <si>
+    <t>Audio-visual recordings and supporting materials</t>
   </si>
 </sst>
 </file>
@@ -4168,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,9 +4203,10 @@
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>332</v>
       </c>
@@ -4191,8 +4216,11 @@
       <c r="G1" s="3" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>329</v>
       </c>
@@ -4202,8 +4230,11 @@
       <c r="G2" s="3" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>329</v>
       </c>
@@ -4213,8 +4244,11 @@
       <c r="G3" s="3" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>330</v>
       </c>
@@ -4224,8 +4258,11 @@
       <c r="G4" s="3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>334</v>
       </c>
@@ -4236,8 +4273,11 @@
       <c r="G5" s="3" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>330</v>
       </c>
@@ -4248,8 +4288,11 @@
       <c r="G6" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>334</v>
       </c>
@@ -4260,8 +4303,11 @@
       <c r="G7" s="3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>335</v>
       </c>
@@ -4272,8 +4318,11 @@
       <c r="G8" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>332</v>
       </c>
@@ -4282,7 +4331,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>332</v>
       </c>
@@ -4291,7 +4340,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>335</v>
       </c>
@@ -4300,7 +4349,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>335</v>
       </c>
@@ -4309,7 +4358,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>332</v>
       </c>
@@ -4318,7 +4367,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>330</v>
       </c>
@@ -4327,7 +4376,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>335</v>
       </c>
@@ -4336,7 +4385,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>332</v>
       </c>

</xml_diff>